<commit_message>
Remove formatting to indicate level of possible automation
This information can still be accessed via version control, but is mainly distracting at this point
</commit_message>
<xml_diff>
--- a/Testing Requirements Summary.xlsx
+++ b/Testing Requirements Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/215cb02a53dcd42a/Mac/Research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="302" documentId="8_{3E13A5A3-BDC1-4AC4-B409-679A99B9269D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2A10F09-355A-43D2-B443-26AA72445295}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36062F39-1CC6-4DC4-B7DD-87DD659E6211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{E12763FB-B22C-4059-84CC-0E30C7790E5B}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{E12763FB-B22C-4059-84CC-0E30C7790E5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
   <si>
     <t>Category</t>
   </si>
@@ -109,9 +107,6 @@
   </si>
   <si>
     <t>Not (easily) able to create</t>
-  </si>
-  <si>
-    <t>Doesn’t currently exists, but could</t>
   </si>
   <si>
     <t>Already exists</t>
@@ -161,109 +156,10 @@
     <t>User requirements are reasonable and feedback is valid</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Metrics from user
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>User feedback</t>
-    </r>
-  </si>
-  <si>
     <t>Incorrect interfaces</t>
   </si>
   <si>
     <t>Requirements not satisfied</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Structure of code modules </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(?)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Knowledge of the modules' interfaces </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(?)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Types of inputs/outputs </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(?)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Typical/default inputs</t>
-    </r>
   </si>
   <si>
     <t>Parameter mismatches
@@ -287,22 +183,6 @@
   <si>
     <t>Specification
 Error checking</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">System tests </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(once implemented)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -352,23 +232,6 @@
     <t>Specific benchmarks from user</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Requirements not satisfied
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Actual metrics</t>
-    </r>
-  </si>
-  <si>
     <t>These are applicable to the "Assets" group of columns and the "Checking Method" and "Reporting" columns</t>
   </si>
   <si>
@@ -381,188 +244,66 @@
 Inputs that result in incorrect behaviour</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Structure of code modules </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(?)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Formal specification of each module </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(?)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Typical/default inputs</t>
-    </r>
-  </si>
-  <si>
     <t>Code for metric reporting</t>
   </si>
   <si>
     <t>?</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Prerequisites for installation
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Required steps to install/run
-Method to check successful installation
-   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Other tests? </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(once implemented)</t>
-    </r>
   </si>
   <si>
     <t>Where the installation failed
 Which tests or functionality couldn't be run</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Formal specification of the program
-User documentation </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(?)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(At least most of) the program code
-Typical/default inputs
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Often random, representative inputs (to test reliability)</t>
-    </r>
-  </si>
-  <si>
     <t>Outputs to sample system inputs
 Outputs to Drasil's typical/default inputs</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">User environment(s)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Method to check successful installation</t>
-    </r>
-  </si>
-  <si>
     <t>---</t>
+  </si>
+  <si>
+    <t>System tests (once implemented)</t>
+  </si>
+  <si>
+    <t>Metrics from user
+User feedback</t>
+  </si>
+  <si>
+    <t>Requirements not satisfied
+Actual metrics</t>
+  </si>
+  <si>
+    <t>User environment(s)
+Method to check successful installation</t>
+  </si>
+  <si>
+    <t>Prerequisites for installation
+Required steps to install/run
+Method to check successful installation
+   Other tests? (once implemented)</t>
+  </si>
+  <si>
+    <t>Structure of code modules
+Formal specification of each module
+Typical/default inputs</t>
+  </si>
+  <si>
+    <t>Structure of code modules
+Knowledge of the modules' interfaces
+Types of inputs/outputs
+Typical/default inputs</t>
+  </si>
+  <si>
+    <t>Formal specification of the program
+User documentation
+(At least most of) the program code
+Typical/default inputs
+Often random, representative inputs (to test reliability)</t>
+  </si>
+  <si>
+    <t>These had been previously used, but we should wait to "fully" understand manual testing before making these classifications</t>
+  </si>
+  <si>
+    <t>Doesn’t currently exist, but could</t>
   </si>
 </sst>
 </file>
@@ -685,12 +426,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -725,72 +465,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1108,248 +838,248 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B80913D-8B48-41BE-9ECA-130A458952EB}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" style="33" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="38.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="12" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="12.84375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="25.69140625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="23.15234375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="38.3828125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3046875" style="16" customWidth="1"/>
+    <col min="7" max="7" width="18.69140625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="16.53515625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="16.69140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.53515625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="25.15234375" style="11" customWidth="1"/>
+    <col min="12" max="12" width="9.69140625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="23" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="15" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="10"/>
-    </row>
-    <row r="2" spans="1:12" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="2" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+    <row r="3" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A4" s="25"/>
+      <c r="B4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A5" s="25"/>
+      <c r="B5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="D5" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A6" s="25"/>
+      <c r="B6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="36" t="s">
+      <c r="F6" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="12" t="s">
+    </row>
+    <row r="7" spans="1:12" s="8" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A7" s="26"/>
+      <c r="B7" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="19" t="s">
+      <c r="J7" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="L7" s="14"/>
+      <c r="K7" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1358,80 +1088,74 @@
     <mergeCell ref="A3:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9064E486-3AB7-4F39-9F8C-DD4DF1A52F7D}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3828125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
         <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved Drasil assets to end of table
Also added some cell contents that are reused
</commit_message>
<xml_diff>
--- a/Testing Requirements Summary.xlsx
+++ b/Testing Requirements Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36062F39-1CC6-4DC4-B7DD-87DD659E6211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA27E9E1-4F16-4059-9D88-4465FBCF2D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{E12763FB-B22C-4059-84CC-0E30C7790E5B}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{E12763FB-B22C-4059-84CC-0E30C7790E5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
   <si>
     <t>Category</t>
   </si>
@@ -46,12 +46,6 @@
     <t>Required Assets</t>
   </si>
   <si>
-    <t>Manual Inputs</t>
-  </si>
-  <si>
-    <t>Manual Outputs</t>
-  </si>
-  <si>
     <t>Checking Method</t>
   </si>
   <si>
@@ -65,12 +59,6 @@
   </si>
   <si>
     <t>Reporting</t>
-  </si>
-  <si>
-    <t>Drasil Inputs</t>
-  </si>
-  <si>
-    <t>Drasil Outputs</t>
   </si>
   <si>
     <t>Knowledge</t>
@@ -140,10 +128,6 @@
 Incompatibility with an environment</t>
   </si>
   <si>
-    <t>Outputs to sample module inputs
-Outputs to Drasil's typical/default inputs</t>
-  </si>
-  <si>
     <t>Confidence in implementation of modules</t>
   </si>
   <si>
@@ -157,9 +141,6 @@
   </si>
   <si>
     <t>Incorrect interfaces</t>
-  </si>
-  <si>
-    <t>Requirements not satisfied</t>
   </si>
   <si>
     <t>Parameter mismatches
@@ -226,9 +207,6 @@
     <t>Not worth it for this testing, but may be added as a result of other testing</t>
   </si>
   <si>
-    <t>Behaviour on errors</t>
-  </si>
-  <si>
     <t>Specific benchmarks from user</t>
   </si>
   <si>
@@ -252,10 +230,6 @@
   <si>
     <t>Where the installation failed
 Which tests or functionality couldn't be run</t>
-  </si>
-  <si>
-    <t>Outputs to sample system inputs
-Outputs to Drasil's typical/default inputs</t>
   </si>
   <si>
     <t>---</t>
@@ -304,6 +278,26 @@
   </si>
   <si>
     <t>Doesn’t currently exist, but could</t>
+  </si>
+  <si>
+    <t>Drasil Assets</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Outputs</t>
+  </si>
+  <si>
+    <t>Outputs to sample module inputs</t>
+  </si>
+  <si>
+    <t>Behaviour on errors
+Outputs to typical/default inputs</t>
+  </si>
+  <si>
+    <t>Requirements not satisfied
+Issues with module specification or implementation</t>
   </si>
 </sst>
 </file>
@@ -431,9 +425,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -442,9 +433,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -475,10 +463,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -516,11 +501,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -838,254 +832,257 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B80913D-8B48-41BE-9ECA-130A458952EB}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="12.84375" style="19" customWidth="1"/>
-    <col min="3" max="3" width="25.69140625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="23.15234375" style="11" customWidth="1"/>
-    <col min="5" max="5" width="38.3828125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3046875" style="16" customWidth="1"/>
-    <col min="7" max="7" width="18.69140625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="16.53515625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="16.69140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.53515625" style="11" customWidth="1"/>
-    <col min="11" max="11" width="25.15234375" style="11" customWidth="1"/>
-    <col min="12" max="12" width="9.69140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="12.84375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="26.15234375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="14.69140625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="18.69140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="16.53515625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="16.69140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.53515625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="25.15234375" style="14" customWidth="1"/>
+    <col min="10" max="10" width="33.15234375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="18.3046875" style="14" customWidth="1"/>
+    <col min="12" max="12" width="9.69140625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="2"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="21" t="s">
+      <c r="A1" s="31"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="22" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="20"/>
+      <c r="L1" s="7"/>
+    </row>
+    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A3" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A4" s="22"/>
+      <c r="B4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A5" s="22"/>
+      <c r="B5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="9"/>
-    </row>
-    <row r="2" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A3" s="24" t="s">
+      <c r="C5" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A6" s="22"/>
+      <c r="B6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="C6" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="6" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A7" s="23"/>
+      <c r="B7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C7" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="28" t="s">
+      <c r="G7" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="J7" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="27" t="s">
+      <c r="K7" s="28" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A4" s="25"/>
-      <c r="B4" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A5" s="25"/>
-      <c r="B5" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="K5" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A6" s="25"/>
-      <c r="B6" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="8" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A7" s="26"/>
-      <c r="B7" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="L7" s="13"/>
+      <c r="L7" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:K1"/>
+  <mergeCells count="4">
+    <mergeCell ref="E1:I1"/>
     <mergeCell ref="A3:A7"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -1096,66 +1093,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9064E486-3AB7-4F39-9F8C-DD4DF1A52F7D}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.3828125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3828125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
-        <v>49</v>
+      <c r="A1" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
-        <v>46</v>
+      <c r="A7" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" s="3" t="s">
-        <v>48</v>
+      <c r="A8" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add initial information about Integration Techniques
Add assumptions for Unit/Integration Testing
Fix Outputs for System Testing
</commit_message>
<xml_diff>
--- a/Testing Requirements Summary.xlsx
+++ b/Testing Requirements Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA27E9E1-4F16-4059-9D88-4465FBCF2D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD688DEA-376D-4AFF-B94F-D6A93178AEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{E12763FB-B22C-4059-84CC-0E30C7790E5B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
   <si>
     <t>Category</t>
   </si>
@@ -148,10 +148,6 @@
   </si>
   <si>
     <t>Issues with module specification or implementation</t>
-  </si>
-  <si>
-    <t>Sample module inputs, including those that are outputs from other modules
-Approach (see Integration Techniques)</t>
   </si>
   <si>
     <t>Confidence in the system as a whole
@@ -298,6 +294,61 @@
   <si>
     <t>Requirements not satisfied
 Issues with module specification or implementation</t>
+  </si>
+  <si>
+    <t>Bottom-up Testing</t>
+  </si>
+  <si>
+    <t>Top-down Testing</t>
+  </si>
+  <si>
+    <t>Sandwich Testing</t>
+  </si>
+  <si>
+    <t>Integration Techniques</t>
+  </si>
+  <si>
+    <t>Big Bang Testing</t>
+  </si>
+  <si>
+    <t>Module hierarchy
+Test drivers
+Sample module inputs</t>
+  </si>
+  <si>
+    <t>Module hierarchy
+Test stubs
+Sample module inputs</t>
+  </si>
+  <si>
+    <t>Module hierarchy
+Sample module inputs</t>
+  </si>
+  <si>
+    <t>Module hierarchy
+Test drivers
+Test stubs
+Target layer (where to meet)
+Sample module inputs</t>
+  </si>
+  <si>
+    <t>Outputs to sample module inputs (from another module)</t>
+  </si>
+  <si>
+    <t>The system has multiple modules (and/or functions?)</t>
+  </si>
+  <si>
+    <t>Outputs to sample system inputs</t>
+  </si>
+  <si>
+    <t>See "Integration Testing"</t>
+  </si>
+  <si>
+    <t>Sample module inputs, including those that are outputs from other modules
+Approach (see "Integration Techniques")</t>
+  </si>
+  <si>
+    <t>Usually "quite challenging and risky", but might be easier and more practical for Drasil</t>
   </si>
 </sst>
 </file>
@@ -337,7 +388,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -416,15 +467,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -462,6 +543,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -471,14 +558,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -489,32 +582,47 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -830,259 +938,342 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B80913D-8B48-41BE-9ECA-130A458952EB}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="12.84375" style="16" customWidth="1"/>
-    <col min="3" max="3" width="26.15234375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="14.69140625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="18.69140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="16.53515625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="16.69140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.53515625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="25.15234375" style="14" customWidth="1"/>
-    <col min="10" max="10" width="33.15234375" style="9" customWidth="1"/>
-    <col min="11" max="11" width="18.3046875" style="14" customWidth="1"/>
-    <col min="12" max="12" width="9.69140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="12.84375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="26.15234375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="19.61328125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="18.69140625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="16.53515625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="16.69140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.53515625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="25.15234375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="33.15234375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="18.3046875" style="13" customWidth="1"/>
+    <col min="12" max="12" width="21" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="31"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="18" t="s">
+    <row r="1" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="21"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="29" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="19" t="s">
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="28"/>
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="20"/>
-      <c r="L1" s="7"/>
-    </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="K2" s="13" t="s">
+      <c r="E3" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A4" s="25"/>
+      <c r="B4" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A3" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="25" t="s">
+      <c r="E4" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="26" t="s">
+    </row>
+    <row r="5" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A5" s="25"/>
+      <c r="B5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A6" s="25"/>
+      <c r="B6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="5" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A7" s="26"/>
+      <c r="B7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" s="25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A4" s="22"/>
-      <c r="B4" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="K4" s="25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A5" s="22"/>
-      <c r="B5" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="K5" s="25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A6" s="22"/>
-      <c r="B6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="24" t="s">
+      <c r="J7" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A8" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="J6" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" s="25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="6" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A7" s="23"/>
-      <c r="B7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="K7" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="11"/>
+      <c r="C8" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="35"/>
+    </row>
+    <row r="9" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A9" s="25"/>
+      <c r="B9" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="36"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="37"/>
+    </row>
+    <row r="10" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A10" s="25"/>
+      <c r="B10" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="36"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="37"/>
+      <c r="L10" s="30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="5" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A11" s="26"/>
+      <c r="B11" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="38"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="A8:A11"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E8:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -1099,24 +1290,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.3828125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3828125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
-        <v>43</v>
+      <c r="A1" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
@@ -1124,15 +1315,15 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
@@ -1140,19 +1331,19 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move general assets from Drasil section
</commit_message>
<xml_diff>
--- a/Testing Requirements Summary.xlsx
+++ b/Testing Requirements Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD688DEA-376D-4AFF-B94F-D6A93178AEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC0A55F-0F38-4C60-BC06-E6D05E8F8322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{E12763FB-B22C-4059-84CC-0E30C7790E5B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
   <si>
     <t>Category</t>
   </si>
@@ -102,19 +102,6 @@
   <si>
     <t>Module coverage
 Incorrect part(s) of modules</t>
-  </si>
-  <si>
-    <t>Sample module inputs</t>
-  </si>
-  <si>
-    <t>Sample system inputs</t>
-  </si>
-  <si>
-    <t>User requirements
-User feedback</t>
-  </si>
-  <si>
-    <t>Installation successful?</t>
   </si>
   <si>
     <t>Do other tests pass in different environments?</t>
@@ -132,9 +119,6 @@
   </si>
   <si>
     <t>Confidence in module interfaces</t>
-  </si>
-  <si>
-    <t>Confidence in the system as a whole</t>
   </si>
   <si>
     <t>User requirements are reasonable and feedback is valid</t>
@@ -231,9 +215,6 @@
     <t>---</t>
   </si>
   <si>
-    <t>System tests (once implemented)</t>
-  </si>
-  <si>
     <t>Metrics from user
 User feedback</t>
   </si>
@@ -242,34 +223,6 @@
 Actual metrics</t>
   </si>
   <si>
-    <t>User environment(s)
-Method to check successful installation</t>
-  </si>
-  <si>
-    <t>Prerequisites for installation
-Required steps to install/run
-Method to check successful installation
-   Other tests? (once implemented)</t>
-  </si>
-  <si>
-    <t>Structure of code modules
-Formal specification of each module
-Typical/default inputs</t>
-  </si>
-  <si>
-    <t>Structure of code modules
-Knowledge of the modules' interfaces
-Types of inputs/outputs
-Typical/default inputs</t>
-  </si>
-  <si>
-    <t>Formal specification of the program
-User documentation
-(At least most of) the program code
-Typical/default inputs
-Often random, representative inputs (to test reliability)</t>
-  </si>
-  <si>
     <t>These had been previously used, but we should wait to "fully" understand manual testing before making these classifications</t>
   </si>
   <si>
@@ -283,13 +236,6 @@
   </si>
   <si>
     <t>Outputs</t>
-  </si>
-  <si>
-    <t>Outputs to sample module inputs</t>
-  </si>
-  <si>
-    <t>Behaviour on errors
-Outputs to typical/default inputs</t>
   </si>
   <si>
     <t>Requirements not satisfied
@@ -332,23 +278,66 @@
 Sample module inputs</t>
   </si>
   <si>
-    <t>Outputs to sample module inputs (from another module)</t>
-  </si>
-  <si>
     <t>The system has multiple modules (and/or functions?)</t>
   </si>
   <si>
-    <t>Outputs to sample system inputs</t>
-  </si>
-  <si>
     <t>See "Integration Testing"</t>
   </si>
   <si>
-    <t>Sample module inputs, including those that are outputs from other modules
+    <t>Usually "quite challenging and risky", but might be easier and more practical for Drasil</t>
+  </si>
+  <si>
+    <t>Structure of code modules
+Formal specification of each module
+Sample module inputs</t>
+  </si>
+  <si>
+    <t>Typical/default inputs</t>
+  </si>
+  <si>
+    <t>Structure of code modules
+Module interfaces
+Types of inputs/outputs
+Sample module inputs, including those that are outputs from other modules
 Approach (see "Integration Techniques")</t>
   </si>
   <si>
-    <t>Usually "quite challenging and risky", but might be easier and more practical for Drasil</t>
+    <t>Outputs to typical/default inputs</t>
+  </si>
+  <si>
+    <t>Outputs to sample module inputs
+Behaviour on errors</t>
+  </si>
+  <si>
+    <t>Outputs to sample system inputs
+Behaviour on errors</t>
+  </si>
+  <si>
+    <t>System tests
+User requirements
+User feedback</t>
+  </si>
+  <si>
+    <t>User environment(s)
+Prerequisites for installation
+Required steps to install/run
+Method to check successful installation
+   Other tests? (once implemented)</t>
+  </si>
+  <si>
+    <t>Formal specification of the program
+User documentation
+(Mostly) complete code
+Sample system inputs
+Random, representative inputs (to test reliability)</t>
+  </si>
+  <si>
+    <t>Confidence in the system as a whole
+Confidence in reliability NFR</t>
+  </si>
+  <si>
+    <t>Outputs to sample module inputs (from another module)
+Behaviour on errors</t>
   </si>
 </sst>
 </file>
@@ -504,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -573,6 +562,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -591,37 +583,52 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -940,17 +947,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B80913D-8B48-41BE-9ECA-130A458952EB}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="12.84375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="26.15234375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="32.84375" style="8" customWidth="1"/>
     <col min="4" max="4" width="19.61328125" style="13" customWidth="1"/>
     <col min="5" max="5" width="18.69140625" style="8" customWidth="1"/>
     <col min="6" max="6" width="16.53515625" style="8" customWidth="1"/>
@@ -965,21 +972,21 @@
     <row r="1" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21"/>
       <c r="B1" s="16"/>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="27" t="s">
+      <c r="D1" s="29"/>
+      <c r="E1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="29"/>
       <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.4">
@@ -990,10 +997,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>4</v>
@@ -1011,260 +1018,268 @@
         <v>7</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>78</v>
+        <v>71</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>64</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I3" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A4" s="25"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="91.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="26"/>
       <c r="B4" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>78</v>
+        <v>71</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>64</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A5" s="25"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="96.45" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="26"/>
       <c r="B5" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A6" s="25"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>52</v>
+      <c r="I6" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>46</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="5" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A7" s="26"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="5" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A7" s="27"/>
       <c r="B7" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A8" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="10"/>
-    </row>
-    <row r="8" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A8" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>68</v>
-      </c>
       <c r="C8" s="8" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E8" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="35"/>
-    </row>
-    <row r="9" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A9" s="25"/>
+      <c r="E8" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="41"/>
+    </row>
+    <row r="9" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A9" s="26"/>
       <c r="B9" s="17" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="37"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="41"/>
     </row>
     <row r="10" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="17" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="37"/>
-      <c r="L10" s="30" t="s">
-        <v>82</v>
+      <c r="E10" s="33"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="13" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="5" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A11" s="26"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="18" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="10"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1295,15 +1310,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -1319,7 +1334,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
@@ -1332,18 +1347,18 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify Results of Testing section to reflect the area in which confidence is increased
</commit_message>
<xml_diff>
--- a/Testing Requirements Summary.xlsx
+++ b/Testing Requirements Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC0A55F-0F38-4C60-BC06-E6D05E8F8322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EB1DC5-21A8-4FBC-A7AE-0BA5E279EE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{E12763FB-B22C-4059-84CC-0E30C7790E5B}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>Assumptions</t>
   </si>
   <si>
-    <t>Results of Testing</t>
-  </si>
-  <si>
     <t>Info from Failure</t>
   </si>
   <si>
@@ -115,12 +112,6 @@
 Incompatibility with an environment</t>
   </si>
   <si>
-    <t>Confidence in implementation of modules</t>
-  </si>
-  <si>
-    <t>Confidence in module interfaces</t>
-  </si>
-  <si>
     <t>User requirements are reasonable and feedback is valid</t>
   </si>
   <si>
@@ -132,14 +123,6 @@
   </si>
   <si>
     <t>Issues with module specification or implementation</t>
-  </si>
-  <si>
-    <t>Confidence in the system as a whole
-Confidence in usability NFR
-Validation</t>
-  </si>
-  <si>
-    <t>Confidence in installability and portability NFRs</t>
   </si>
   <si>
     <t>Specification
@@ -332,12 +315,31 @@
 Random, representative inputs (to test reliability)</t>
   </si>
   <si>
-    <t>Confidence in the system as a whole
-Confidence in reliability NFR</t>
-  </si>
-  <si>
     <t>Outputs to sample module inputs (from another module)
 Behaviour on errors</t>
+  </si>
+  <si>
+    <t>Module correctness</t>
+  </si>
+  <si>
+    <t>Module interface correctness</t>
+  </si>
+  <si>
+    <t>System correctness
+Reliability</t>
+  </si>
+  <si>
+    <t>System correctness
+Usability
+Validation</t>
+  </si>
+  <si>
+    <t>Installability
+Portability</t>
+  </si>
+  <si>
+    <t>Results of Testing
+(Area of Confidence)</t>
   </si>
 </sst>
 </file>
@@ -951,7 +953,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8:I11"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -961,7 +963,7 @@
     <col min="4" max="4" width="19.61328125" style="13" customWidth="1"/>
     <col min="5" max="5" width="18.69140625" style="8" customWidth="1"/>
     <col min="6" max="6" width="16.53515625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="16.69140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.07421875" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.53515625" style="8" customWidth="1"/>
     <col min="9" max="9" width="25.15234375" style="13" customWidth="1"/>
     <col min="10" max="10" width="33.15234375" style="8" customWidth="1"/>
@@ -977,19 +979,19 @@
       </c>
       <c r="D1" s="29"/>
       <c r="E1" s="28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
       <c r="H1" s="28"/>
       <c r="I1" s="29"/>
       <c r="J1" s="28" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="K1" s="29"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
@@ -997,10 +999,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>4</v>
@@ -1009,207 +1011,207 @@
         <v>3</v>
       </c>
       <c r="G2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>7</v>
-      </c>
       <c r="J2" s="11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="91.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="26"/>
       <c r="B4" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="I4" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="96.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="26"/>
       <c r="B5" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A6" s="26"/>
       <c r="B6" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I6" s="37" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J6" s="39" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="5" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A7" s="27"/>
       <c r="B7" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>24</v>
-      </c>
       <c r="I7" s="15" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="K7" s="38" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="L7" s="10"/>
     </row>
     <row r="8" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A8" s="25" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="31" t="s">
         <v>60</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>65</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="32"/>
@@ -1222,13 +1224,13 @@
     <row r="9" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A9" s="26"/>
       <c r="B9" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="D9" s="13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E9" s="33"/>
       <c r="F9" s="34"/>
@@ -1242,13 +1244,13 @@
     <row r="10" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A10" s="26"/>
       <c r="B10" s="17" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E10" s="33"/>
       <c r="F10" s="34"/>
@@ -1258,19 +1260,19 @@
       <c r="J10" s="39"/>
       <c r="K10" s="45"/>
       <c r="L10" s="13" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="5" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A11" s="27"/>
       <c r="B11" s="18" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E11" s="35"/>
       <c r="F11" s="36"/>
@@ -1310,55 +1312,55 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add initial notes on Test Oracles
Correct 'Behaviour of errors' as an output throughout
</commit_message>
<xml_diff>
--- a/Testing Requirements Summary.xlsx
+++ b/Testing Requirements Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EB1DC5-21A8-4FBC-A7AE-0BA5E279EE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9117E8A7-4EE2-4DE2-A347-10BC2B27F1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{E12763FB-B22C-4059-84CC-0E30C7790E5B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="111">
   <si>
     <t>Category</t>
   </si>
@@ -221,6 +221,9 @@
     <t>Outputs</t>
   </si>
   <si>
+    <t>Outputs to sample module inputs</t>
+  </si>
+  <si>
     <t>Requirements not satisfied
 Issues with module specification or implementation</t>
   </si>
@@ -261,7 +264,13 @@
 Sample module inputs</t>
   </si>
   <si>
+    <t>Outputs to sample module inputs (from another module)</t>
+  </si>
+  <si>
     <t>The system has multiple modules (and/or functions?)</t>
+  </si>
+  <si>
+    <t>Outputs to sample system inputs</t>
   </si>
   <si>
     <t>See "Integration Testing"</t>
@@ -288,14 +297,6 @@
     <t>Outputs to typical/default inputs</t>
   </si>
   <si>
-    <t>Outputs to sample module inputs
-Behaviour on errors</t>
-  </si>
-  <si>
-    <t>Outputs to sample system inputs
-Behaviour on errors</t>
-  </si>
-  <si>
     <t>System tests
 User requirements
 User feedback</t>
@@ -315,20 +316,6 @@
 Random, representative inputs (to test reliability)</t>
   </si>
   <si>
-    <t>Outputs to sample module inputs (from another module)
-Behaviour on errors</t>
-  </si>
-  <si>
-    <t>Module correctness</t>
-  </si>
-  <si>
-    <t>Module interface correctness</t>
-  </si>
-  <si>
-    <t>System correctness
-Reliability</t>
-  </si>
-  <si>
     <t>System correctness
 Usability
 Validation</t>
@@ -340,6 +327,132 @@
   <si>
     <t>Results of Testing
 (Area of Confidence)</t>
+  </si>
+  <si>
+    <t>Specified Test Oracle</t>
+  </si>
+  <si>
+    <t>Derived Test Oracle</t>
+  </si>
+  <si>
+    <t>Pseudo-oracle</t>
+  </si>
+  <si>
+    <t>Implict Test Oracle</t>
+  </si>
+  <si>
+    <t>Lack of an Automated Test Oracle</t>
+  </si>
+  <si>
+    <t>Test Oracles</t>
+  </si>
+  <si>
+    <t>Formal specification of the program
+Sample inputs</t>
+  </si>
+  <si>
+    <t>Outputs to sample inputs</t>
+  </si>
+  <si>
+    <t>Issues with specification or implementation</t>
+  </si>
+  <si>
+    <t>Issues with specification or implementation
+Inconsistency between artifacts</t>
+  </si>
+  <si>
+    <t>Incorrect parts of code</t>
+  </si>
+  <si>
+    <t>Incorrect parts of code
+Discrepancies</t>
+  </si>
+  <si>
+    <t>A type of derived test oracle</t>
+  </si>
+  <si>
+    <t>All artifacts are maintained</t>
+  </si>
+  <si>
+    <t>Correctness
+Traceability
+Maintainability</t>
+  </si>
+  <si>
+    <t>Multiple versions of the program</t>
+  </si>
+  <si>
+    <t>Human-generated sample input (e.g., through historical use or "many eyes")</t>
+  </si>
+  <si>
+    <t>Error checking</t>
+  </si>
+  <si>
+    <t>Common program faults</t>
+  </si>
+  <si>
+    <t>Any artifacts that allow for tests to be generated: previous implementations, documentation, existing test cases, APIs, invariants, etc.
+Sample inputs</t>
+  </si>
+  <si>
+    <t>Robustness</t>
+  </si>
+  <si>
+    <t>System correctness
+Robustness
+Reliability</t>
+  </si>
+  <si>
+    <t>Module correctness
+Robustness</t>
+  </si>
+  <si>
+    <t>Module interface correctness
+Robustness</t>
+  </si>
+  <si>
+    <t>Correctness
+Robustness</t>
+  </si>
+  <si>
+    <t>Correctness
+Robustness
+Traceability
+Maintainability</t>
+  </si>
+  <si>
+    <t>Consistency</t>
+  </si>
+  <si>
+    <t>The versions provide the same functionality</t>
+  </si>
+  <si>
+    <t>The human-generated input is correct and useful</t>
+  </si>
+  <si>
+    <t>Formal specification can be translated into meaningful test cases</t>
+  </si>
+  <si>
+    <t>Whether or not the programs produce the same (or similar) results</t>
+  </si>
+  <si>
+    <t>Issues with one (or more) implementations</t>
+  </si>
+  <si>
+    <t>Specification
+Error checking
+Consistency</t>
+  </si>
+  <si>
+    <t>Hazard not accounted for</t>
+  </si>
+  <si>
+    <t>Reliability
+Robustness</t>
+  </si>
+  <si>
+    <t>Incorrect parts of code
+Inputs that result in incorrect behaviour</t>
   </si>
 </sst>
 </file>
@@ -495,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -510,21 +623,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -564,6 +665,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -615,12 +719,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -632,6 +730,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -947,344 +1057,485 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B80913D-8B48-41BE-9ECA-130A458952EB}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="12.84375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="32.84375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="19.61328125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="18.69140625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="16.53515625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="18.07421875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.53515625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="25.15234375" style="13" customWidth="1"/>
-    <col min="10" max="10" width="33.15234375" style="8" customWidth="1"/>
-    <col min="11" max="11" width="18.3046875" style="13" customWidth="1"/>
-    <col min="12" max="12" width="21" style="9" customWidth="1"/>
+    <col min="2" max="2" width="12.84375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="32.84375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="19.61328125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="18.69140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.53515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="18.07421875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.53515625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="25.15234375" style="9" customWidth="1"/>
+    <col min="10" max="10" width="33.15234375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="18.3046875" style="9" customWidth="1"/>
+    <col min="12" max="12" width="21" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="21"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="30" t="s">
+    <row r="1" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="17"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="28" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="28" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="6"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="43"/>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A3" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
+      <c r="A4" s="23"/>
+      <c r="B4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A5" s="23"/>
+      <c r="B5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A6" s="23"/>
+      <c r="B6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="5" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A7" s="24"/>
+      <c r="B7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="45"/>
+    </row>
+    <row r="8" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A8" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A9" s="23"/>
+      <c r="B9" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A10" s="23"/>
+      <c r="B10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="5" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A11" s="24"/>
+      <c r="B11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A12" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A13" s="42"/>
+      <c r="B13" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A14" s="42"/>
+      <c r="B14" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A3" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="91.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="26"/>
-      <c r="B4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="96.45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="26"/>
-      <c r="B5" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A6" s="26"/>
-      <c r="B6" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="39" t="s">
+      <c r="C14" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="L14" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A15" s="42"/>
+      <c r="B15" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="5" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A7" s="27"/>
-      <c r="B7" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="20" t="s">
+      <c r="F15" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A16" s="24"/>
+      <c r="B16" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" s="10"/>
-    </row>
-    <row r="8" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A8" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="41"/>
-    </row>
-    <row r="9" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A9" s="26"/>
-      <c r="B9" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="33"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="41"/>
-    </row>
-    <row r="10" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A10" s="26"/>
-      <c r="B10" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="5" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A11" s="27"/>
-      <c r="B11" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="42"/>
+      <c r="E16" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J16" s="10"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A12:A16"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="A3:A7"/>

</xml_diff>

<commit_message>
Minor formatting fix to summary spreadsheet
</commit_message>
<xml_diff>
--- a/Testing Requirements Summary.xlsx
+++ b/Testing Requirements Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9117E8A7-4EE2-4DE2-A347-10BC2B27F1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEA111B-6D31-40B9-978F-BAB88E34A40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{E12763FB-B22C-4059-84CC-0E30C7790E5B}"/>
   </bookViews>
@@ -608,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -671,6 +671,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -706,42 +733,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1060,10 +1051,10 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1084,22 +1075,22 @@
     <row r="1" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="17"/>
       <c r="B1" s="12"/>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="25" t="s">
+      <c r="D1" s="35"/>
+      <c r="E1" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="25" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="26"/>
-      <c r="L1" s="43"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="28"/>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A2" s="18" t="s">
@@ -1135,12 +1126,12 @@
       <c r="K2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="44" t="s">
+      <c r="L2" s="29" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -1175,7 +1166,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
-      <c r="A4" s="23"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="13" t="s">
         <v>10</v>
       </c>
@@ -1208,7 +1199,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A5" s="23"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="13" t="s">
         <v>11</v>
       </c>
@@ -1241,7 +1232,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A6" s="23"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1263,10 +1254,10 @@
       <c r="H6" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="23" t="s">
         <v>41</v>
       </c>
       <c r="K6" s="9" t="s">
@@ -1274,7 +1265,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" s="5" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A7" s="24"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="14" t="s">
         <v>13</v>
       </c>
@@ -1299,16 +1290,16 @@
       <c r="I7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="35" t="s">
+      <c r="J7" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="35" t="s">
+      <c r="K7" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="L7" s="45"/>
+      <c r="L7" s="30"/>
     </row>
     <row r="8" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="31" t="s">
         <v>54</v>
       </c>
       <c r="B8" s="13" t="s">
@@ -1320,19 +1311,19 @@
       <c r="D8" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="39"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="25"/>
       <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A9" s="23"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="13" t="s">
         <v>52</v>
       </c>
@@ -1342,17 +1333,17 @@
       <c r="D9" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="40"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="26"/>
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A10" s="23"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="13" t="s">
         <v>55</v>
       </c>
@@ -1362,19 +1353,19 @@
       <c r="D10" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="40"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="26"/>
       <c r="L10" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="5" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A11" s="24"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="14" t="s">
         <v>53</v>
       </c>
@@ -1384,17 +1375,17 @@
       <c r="D11" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="27"/>
       <c r="K11" s="16"/>
       <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="31" t="s">
         <v>80</v>
       </c>
       <c r="B12" s="13" t="s">
@@ -1423,7 +1414,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A13" s="42"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="13" t="s">
         <v>76</v>
       </c>
@@ -1450,7 +1441,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A14" s="42"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="13" t="s">
         <v>77</v>
       </c>
@@ -1480,14 +1471,14 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A15" s="42"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="13" t="s">
         <v>78</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="26" t="s">
         <v>41</v>
       </c>
       <c r="F15" s="6" t="s">
@@ -1504,7 +1495,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A16" s="24"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="14" t="s">
         <v>79</v>
       </c>
@@ -1523,7 +1514,7 @@
       <c r="G16" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="10" t="s">
         <v>83</v>
       </c>
       <c r="I16" s="11" t="s">
@@ -1531,7 +1522,7 @@
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="11"/>
-      <c r="L16" s="45"/>
+      <c r="L16" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Add subject column and populate for testing stages
</commit_message>
<xml_diff>
--- a/Testing Requirements Summary.xlsx
+++ b/Testing Requirements Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEA111B-6D31-40B9-978F-BAB88E34A40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2426CE28-8652-4D24-A17A-71B6C3902CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{E12763FB-B22C-4059-84CC-0E30C7790E5B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="117">
   <si>
     <t>Category</t>
   </si>
@@ -279,19 +279,7 @@
     <t>Usually "quite challenging and risky", but might be easier and more practical for Drasil</t>
   </si>
   <si>
-    <t>Structure of code modules
-Formal specification of each module
-Sample module inputs</t>
-  </si>
-  <si>
     <t>Typical/default inputs</t>
-  </si>
-  <si>
-    <t>Structure of code modules
-Module interfaces
-Types of inputs/outputs
-Sample module inputs, including those that are outputs from other modules
-Approach (see "Integration Techniques")</t>
   </si>
   <si>
     <t>Outputs to typical/default inputs</t>
@@ -309,13 +297,6 @@
    Other tests? (once implemented)</t>
   </si>
   <si>
-    <t>Formal specification of the program
-User documentation
-(Mostly) complete code
-Sample system inputs
-Random, representative inputs (to test reliability)</t>
-  </si>
-  <si>
     <t>System correctness
 Usability
 Validation</t>
@@ -453,6 +434,42 @@
   <si>
     <t>Incorrect parts of code
 Inputs that result in incorrect behaviour</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Modules</t>
+  </si>
+  <si>
+    <t>Formal specification of each module
+Sample module inputs</t>
+  </si>
+  <si>
+    <t>Module interfaces</t>
+  </si>
+  <si>
+    <t>Types of inputs/outputs
+Sample module inputs, including those that are outputs from other modules
+Approach (see "Integration Techniques")</t>
+  </si>
+  <si>
+    <t>Formal specification of the program
+User documentation
+Sample system inputs
+Random, representative inputs (to test reliability)</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Code
+   (most or all)</t>
+  </si>
+  <si>
+    <t>Code
+Documentation
+   (installation)</t>
   </si>
 </sst>
 </file>
@@ -608,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -733,6 +750,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1048,51 +1074,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B80913D-8B48-41BE-9ECA-130A458952EB}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="12.84375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="32.84375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="19.61328125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="18.69140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.53515625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="18.07421875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.53515625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="25.15234375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="33.15234375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="18.3046875" style="9" customWidth="1"/>
-    <col min="12" max="12" width="21" style="20" customWidth="1"/>
+    <col min="3" max="3" width="14.07421875" style="44" customWidth="1"/>
+    <col min="4" max="4" width="32.84375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.61328125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="18.69140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="16.53515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="18.07421875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.53515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="25.15234375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="33.15234375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="18.3046875" style="9" customWidth="1"/>
+    <col min="13" max="13" width="21" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="17"/>
       <c r="B1" s="12"/>
       <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="34" t="s">
+      <c r="D1" s="43"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="34"/>
       <c r="G1" s="34"/>
       <c r="H1" s="34"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="34" t="s">
+      <c r="I1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="35"/>
-      <c r="L1" s="28"/>
-    </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L1" s="35"/>
+      <c r="M1" s="28"/>
+    </row>
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -1100,439 +1128,459 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="H2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="M2" s="29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A3" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="L3" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="K3" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="116.6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A4" s="32"/>
       <c r="B4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F4" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>98</v>
-      </c>
       <c r="H4" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A5" s="32"/>
       <c r="B5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="F5" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>96</v>
-      </c>
       <c r="H5" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="K5" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A6" s="32"/>
       <c r="B6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="K6" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="L6" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="5" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" s="5" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A7" s="33"/>
       <c r="B7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="H7" s="10" t="s">
+      <c r="I7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="J7" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>41</v>
       </c>
       <c r="K7" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="L7" s="30"/>
-    </row>
-    <row r="8" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="L7" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="30"/>
+    </row>
+    <row r="8" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A8" s="31" t="s">
         <v>54</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="F8" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="38"/>
       <c r="G8" s="38"/>
       <c r="H8" s="38"/>
       <c r="I8" s="38"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="J8" s="38"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A9" s="32"/>
       <c r="B9" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="40"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="40"/>
       <c r="H9" s="40"/>
       <c r="I9" s="40"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="9"/>
-    </row>
-    <row r="10" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="J9" s="40"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A10" s="32"/>
       <c r="B10" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="40"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="40"/>
       <c r="H10" s="40"/>
       <c r="I10" s="40"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="9" t="s">
+      <c r="J10" s="40"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="5" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" s="5" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A11" s="33"/>
       <c r="B11" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="45"/>
+      <c r="D11" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="42"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="42"/>
       <c r="H11" s="42"/>
       <c r="I11" s="42"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="11"/>
-    </row>
-    <row r="12" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="J11" s="42"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="11"/>
+    </row>
+    <row r="12" spans="1:13" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A12" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="9" t="s">
+      <c r="J12" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A13" s="32"/>
       <c r="B13" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>88</v>
+        <v>73</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+        <v>97</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A14" s="32"/>
       <c r="B14" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E14" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>102</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="I14" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="L14" s="20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="I14" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="M14" s="20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A15" s="32"/>
       <c r="B15" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="G15" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="I15" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A16" s="33"/>
       <c r="B16" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="45"/>
+      <c r="D16" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>103</v>
-      </c>
       <c r="F16" s="10" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="30"/>
+        <v>106</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="K16" s="10"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A8:A11"/>
-    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="F1:J1"/>
     <mergeCell ref="A3:A7"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E8:I11"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="F8:J11"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Add harness, checking method, and assumption columns; start populating them
</commit_message>
<xml_diff>
--- a/Testing Requirements Summary.xlsx
+++ b/Testing Requirements Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2426CE28-8652-4D24-A17A-71B6C3902CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356E0BC9-E51C-4912-BF9A-6E6E38A1072D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{E12763FB-B22C-4059-84CC-0E30C7790E5B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="117">
   <si>
     <t>Category</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>Reporting</t>
-  </si>
-  <si>
-    <t>Knowledge</t>
   </si>
   <si>
     <t>Testing Stage</t>
@@ -110,9 +107,6 @@
     <t>Incorrect steps for installation
 Missing prequisites
 Incompatibility with an environment</t>
-  </si>
-  <si>
-    <t>User requirements are reasonable and feedback is valid</t>
   </si>
   <si>
     <t>Incorrect interfaces</t>
@@ -198,10 +192,6 @@
     <t>---</t>
   </si>
   <si>
-    <t>Metrics from user
-User feedback</t>
-  </si>
-  <si>
     <t>Requirements not satisfied
 Actual metrics</t>
   </si>
@@ -237,33 +227,13 @@
     <t>Sandwich Testing</t>
   </si>
   <si>
-    <t>Integration Techniques</t>
-  </si>
-  <si>
     <t>Big Bang Testing</t>
-  </si>
-  <si>
-    <t>Module hierarchy
-Test drivers
-Sample module inputs</t>
-  </si>
-  <si>
-    <t>Module hierarchy
-Test stubs
-Sample module inputs</t>
   </si>
   <si>
     <t>Module hierarchy
 Sample module inputs</t>
   </si>
   <si>
-    <t>Module hierarchy
-Test drivers
-Test stubs
-Target layer (where to meet)
-Sample module inputs</t>
-  </si>
-  <si>
     <t>Outputs to sample module inputs (from another module)</t>
   </si>
   <si>
@@ -283,11 +253,6 @@
   </si>
   <si>
     <t>Outputs to typical/default inputs</t>
-  </si>
-  <si>
-    <t>System tests
-User requirements
-User feedback</t>
   </si>
   <si>
     <t>User environment(s)
@@ -297,11 +262,6 @@
    Other tests? (once implemented)</t>
   </si>
   <si>
-    <t>System correctness
-Usability
-Validation</t>
-  </si>
-  <si>
     <t>Installability
 Portability</t>
   </si>
@@ -377,19 +337,6 @@
   </si>
   <si>
     <t>Robustness</t>
-  </si>
-  <si>
-    <t>System correctness
-Robustness
-Reliability</t>
-  </si>
-  <si>
-    <t>Module correctness
-Robustness</t>
-  </si>
-  <si>
-    <t>Module interface correctness
-Robustness</t>
   </si>
   <si>
     <t>Correctness
@@ -460,9 +407,6 @@
 Random, representative inputs (to test reliability)</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>Code
    (most or all)</t>
   </si>
@@ -470,6 +414,58 @@
     <t>Code
 Documentation
    (installation)</t>
+  </si>
+  <si>
+    <t>Harness</t>
+  </si>
+  <si>
+    <t>System tests
+User requirements</t>
+  </si>
+  <si>
+    <t>User feedback
+   (Qualitative/quantitative)</t>
+  </si>
+  <si>
+    <t>Code
+Documentation
+   (requirements)</t>
+  </si>
+  <si>
+    <t>Correctness
+Robustness
+Reliability</t>
+  </si>
+  <si>
+    <t>Correctness
+Usability
+Validation</t>
+  </si>
+  <si>
+    <t>User requirements are reasonable
+User feedback is valid</t>
+  </si>
+  <si>
+    <t>Knowledge Gained</t>
+  </si>
+  <si>
+    <t>Test drivers</t>
+  </si>
+  <si>
+    <t>Test stubs</t>
+  </si>
+  <si>
+    <t>Module hierarchy
+Target layer (where to meet)
+Sample module inputs</t>
+  </si>
+  <si>
+    <t>Test drivers
+Test stubs</t>
+  </si>
+  <si>
+    <t>Integration Techniques
+(applied to the system)</t>
   </si>
 </sst>
 </file>
@@ -509,7 +505,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -589,17 +585,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -625,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -667,9 +652,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -685,25 +667,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -733,19 +703,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -759,6 +720,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1074,513 +1071,543 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B80913D-8B48-41BE-9ECA-130A458952EB}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="12.84375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="14.07421875" style="44" customWidth="1"/>
+    <col min="3" max="3" width="14.07421875" style="36" customWidth="1"/>
     <col min="4" max="4" width="32.84375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.61328125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="18.69140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="16.53515625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="18.07421875" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.53515625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="25.15234375" style="9" customWidth="1"/>
-    <col min="11" max="11" width="33.15234375" style="6" customWidth="1"/>
-    <col min="12" max="12" width="18.3046875" style="9" customWidth="1"/>
-    <col min="13" max="13" width="21" style="20" customWidth="1"/>
+    <col min="5" max="5" width="19.61328125" style="38" customWidth="1"/>
+    <col min="6" max="6" width="22.3828125" style="38" customWidth="1"/>
+    <col min="7" max="7" width="19.61328125" style="38" customWidth="1"/>
+    <col min="8" max="8" width="20.3046875" style="38" customWidth="1"/>
+    <col min="9" max="9" width="18.07421875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.53515625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="25.15234375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="33.15234375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="18.3046875" style="9" customWidth="1"/>
+    <col min="14" max="14" width="21" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="17"/>
+    <row r="1" spans="1:14" s="18" customFormat="1" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="16"/>
       <c r="B1" s="12"/>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="43"/>
+      <c r="D1" s="35"/>
       <c r="E1" s="35"/>
-      <c r="F1" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="35"/>
-      <c r="M1" s="28"/>
-    </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A2" s="18" t="s">
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="30"/>
+      <c r="N1" s="23"/>
+    </row>
+    <row r="2" spans="1:14" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A4" s="27"/>
+      <c r="B4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A5" s="27"/>
+      <c r="B5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="J5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A6" s="27"/>
+      <c r="B6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="K6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="5" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A7" s="28"/>
+      <c r="B7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="39"/>
+      <c r="H7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="25"/>
+    </row>
+    <row r="8" spans="1:14" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A8" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="C8" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="9"/>
+    </row>
+    <row r="9" spans="1:14" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A9" s="27"/>
+      <c r="B9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="47"/>
+      <c r="D9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="42"/>
+      <c r="G9" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="H9" s="44"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="9"/>
+    </row>
+    <row r="10" spans="1:14" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A10" s="27"/>
+      <c r="B10" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="47"/>
+      <c r="D10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="42"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A11" s="28"/>
+      <c r="B11" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="48"/>
+      <c r="D11" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="34"/>
+      <c r="G11" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="H11" s="45"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="11"/>
+    </row>
+    <row r="12" spans="1:14" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A12" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A3" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="K12" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A13" s="27"/>
+      <c r="B13" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A14" s="27"/>
+      <c r="B14" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A15" s="27"/>
+      <c r="B15" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="40"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A16" s="28"/>
+      <c r="B16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="39"/>
+      <c r="H16" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A4" s="32"/>
-      <c r="B4" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="6" t="s">
+      <c r="J16" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A5" s="32"/>
-      <c r="B5" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A6" s="32"/>
-      <c r="B6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="5" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A7" s="33"/>
-      <c r="B7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" s="30"/>
-    </row>
-    <row r="8" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A8" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="9"/>
-    </row>
-    <row r="9" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A9" s="32"/>
-      <c r="B9" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="9"/>
-    </row>
-    <row r="10" spans="1:13" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A10" s="32"/>
-      <c r="B10" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="5" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A11" s="33"/>
-      <c r="B11" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="11"/>
-    </row>
-    <row r="12" spans="1:13" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A12" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A13" s="32"/>
-      <c r="B13" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A14" s="32"/>
-      <c r="B14" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="M14" s="20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A15" s="32"/>
-      <c r="B15" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A16" s="33"/>
-      <c r="B16" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="K16" s="10"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="30"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A8:A11"/>
-    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="I1:K1"/>
     <mergeCell ref="A3:A7"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="F8:J11"/>
-    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="I8:K11"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="C8:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -1602,55 +1629,55 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
         <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add initial pass of static black-box testing
</commit_message>
<xml_diff>
--- a/Testing Requirements Summary.xlsx
+++ b/Testing Requirements Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356E0BC9-E51C-4912-BF9A-6E6E38A1072D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D462170-FFD6-4937-B837-58356069BFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{E12763FB-B22C-4059-84CC-0E30C7790E5B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="133">
   <si>
     <t>Category</t>
   </si>
@@ -466,6 +466,69 @@
   <si>
     <t>Integration Techniques
 (applied to the system)</t>
+  </si>
+  <si>
+    <t>Terminology Checklist</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>List of potentially ambiguous words</t>
+  </si>
+  <si>
+    <t>Whether or not any exist in the documentation</t>
+  </si>
+  <si>
+    <t>Static Black-Box</t>
+  </si>
+  <si>
+    <t>Unambiguity
+Verifiability</t>
+  </si>
+  <si>
+    <t>Areas of the document to be more precise with</t>
+  </si>
+  <si>
+    <t>Which words occur and where</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Do the words appear?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Context-specific uses</t>
+    </r>
+  </si>
+  <si>
+    <t>Coverage-Based Testing</t>
+  </si>
+  <si>
+    <t>Specification</t>
+  </si>
+  <si>
+    <t>Requirements depicted as a graph</t>
+  </si>
+  <si>
+    <t>Test cases based on relationships between requirements</t>
+  </si>
+  <si>
+    <t>"It can be difficult to assess whether a set of equivalence classes are truly equivalent"</t>
+  </si>
+  <si>
+    <t>Every instance of one of these words has the potential to be ambiguous (although it might not be)</t>
+  </si>
+  <si>
+    <t>Script to search for words</t>
   </si>
 </sst>
 </file>
@@ -610,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -755,6 +818,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1071,13 +1137,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B80913D-8B48-41BE-9ECA-130A458952EB}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1085,10 +1151,10 @@
     <col min="2" max="2" width="12.84375" style="13" customWidth="1"/>
     <col min="3" max="3" width="14.07421875" style="36" customWidth="1"/>
     <col min="4" max="4" width="32.84375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.61328125" style="38" customWidth="1"/>
+    <col min="5" max="5" width="21.15234375" style="38" customWidth="1"/>
     <col min="6" max="6" width="22.3828125" style="38" customWidth="1"/>
     <col min="7" max="7" width="19.61328125" style="38" customWidth="1"/>
-    <col min="8" max="8" width="20.3046875" style="38" customWidth="1"/>
+    <col min="8" max="8" width="20.3046875" style="9" customWidth="1"/>
     <col min="9" max="9" width="18.07421875" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.53515625" style="6" customWidth="1"/>
     <col min="11" max="11" width="25.15234375" style="9" customWidth="1"/>
@@ -1553,7 +1619,6 @@
         <v>80</v>
       </c>
       <c r="G15" s="40"/>
-      <c r="H15" s="9"/>
       <c r="I15" s="6" t="s">
         <v>83</v>
       </c>
@@ -1596,8 +1661,70 @@
       <c r="M16" s="11"/>
       <c r="N16" s="25"/>
     </row>
+    <row r="17" spans="1:14" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A17" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E17" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="5" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A18" s="50"/>
+      <c r="B18" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="25" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A17:A18"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="I1:K1"/>

</xml_diff>

<commit_message>
Start adding dynamic black-box testing
</commit_message>
<xml_diff>
--- a/Testing Requirements Summary.xlsx
+++ b/Testing Requirements Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D462170-FFD6-4937-B837-58356069BFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB0625E-8034-43D8-A9AA-C70238E13200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{E12763FB-B22C-4059-84CC-0E30C7790E5B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="162">
   <si>
     <t>Category</t>
   </si>
@@ -407,6 +407,9 @@
 Random, representative inputs (to test reliability)</t>
   </si>
   <si>
+    <t>Code</t>
+  </si>
+  <si>
     <t>Code
    (most or all)</t>
   </si>
@@ -475,9 +478,6 @@
   </si>
   <si>
     <t>List of potentially ambiguous words</t>
-  </si>
-  <si>
-    <t>Whether or not any exist in the documentation</t>
   </si>
   <si>
     <t>Static Black-Box</t>
@@ -528,7 +528,100 @@
     <t>Every instance of one of these words has the potential to be ambiguous (although it might not be)</t>
   </si>
   <si>
-    <t>Script to search for words</t>
+    <t>Exploratory Testing</t>
+  </si>
+  <si>
+    <t>A specification is not available</t>
+  </si>
+  <si>
+    <t>Knowledge of the features
+Tests for discovered features</t>
+  </si>
+  <si>
+    <t>Manual exploration (e.g., trial-and-error)</t>
+  </si>
+  <si>
+    <t>Understandability?</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Which features have bugs (and what they are)</t>
+  </si>
+  <si>
+    <t>Equivalence Partitioning/Classing</t>
+  </si>
+  <si>
+    <t>Tests?</t>
+  </si>
+  <si>
+    <t>Possible values</t>
+  </si>
+  <si>
+    <t>The most efficient values to test</t>
+  </si>
+  <si>
+    <t>Not sure that this fits into this chart</t>
+  </si>
+  <si>
+    <t>Boundary Condition Testing</t>
+  </si>
+  <si>
+    <t>A type of data testing</t>
+  </si>
+  <si>
+    <t>A type of boundary condition testing</t>
+  </si>
+  <si>
+    <t>Constraints/limits on values</t>
+  </si>
+  <si>
+    <t>Desired handling of edge cases/invalid values</t>
+  </si>
+  <si>
+    <t>Edge cases aren't correctly handled</t>
+  </si>
+  <si>
+    <t>Which constraints are not dealt with
+Which edge cases lead to incorrect behaviour</t>
+  </si>
+  <si>
+    <t>Buffer Overrun Testing</t>
+  </si>
+  <si>
+    <t>Whether or not any exist</t>
+  </si>
+  <si>
+    <t>Searching script</t>
+  </si>
+  <si>
+    <t>Do the functions appear?
+???</t>
+  </si>
+  <si>
+    <t>Unsafe string functions in the given language</t>
+  </si>
+  <si>
+    <t>The code's language has unsafe functions for storing data
+It is never appropriate to use these unsafe functions</t>
+  </si>
+  <si>
+    <t>Areas where data saving needs to be more safe</t>
+  </si>
+  <si>
+    <t>Which unsafe functions are used, where, and their safe counterparts
+Where data is written with insufficient space</t>
+  </si>
+  <si>
+    <t>Whether or not any unsafe string functions are used
+If any data is written with insufficient space</t>
+  </si>
+  <si>
+    <t>Dynamic Black-Box</t>
+  </si>
+  <si>
+    <t>Manual (by a stakeholder)</t>
   </si>
 </sst>
 </file>
@@ -673,7 +766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -729,6 +822,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1137,24 +1233,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B80913D-8B48-41BE-9ECA-130A458952EB}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="12.84375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="14.07421875" style="36" customWidth="1"/>
+    <col min="2" max="2" width="18" style="13" customWidth="1"/>
+    <col min="3" max="3" width="14.07421875" style="37" customWidth="1"/>
     <col min="4" max="4" width="32.84375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="21.15234375" style="38" customWidth="1"/>
-    <col min="6" max="6" width="22.3828125" style="38" customWidth="1"/>
-    <col min="7" max="7" width="19.61328125" style="38" customWidth="1"/>
-    <col min="8" max="8" width="20.3046875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="23.53515625" style="39" customWidth="1"/>
+    <col min="6" max="6" width="22.3828125" style="39" customWidth="1"/>
+    <col min="7" max="7" width="19.61328125" style="39" customWidth="1"/>
+    <col min="8" max="8" width="25.84375" style="9" customWidth="1"/>
     <col min="9" max="9" width="18.07421875" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.53515625" style="6" customWidth="1"/>
     <col min="11" max="11" width="25.15234375" style="9" customWidth="1"/>
@@ -1166,24 +1262,24 @@
     <row r="1" spans="1:14" s="18" customFormat="1" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="16"/>
       <c r="B1" s="12"/>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="J1" s="29"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="29" t="s">
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="30"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="30"/>
-      <c r="N1" s="23"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="24"/>
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A2" s="17" t="s">
@@ -1205,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>4</v>
@@ -1225,24 +1321,24 @@
       <c r="M2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="37" t="s">
         <v>97</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="39" t="s">
         <v>46</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -1268,17 +1364,17 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A4" s="27"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="37" t="s">
         <v>99</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="39" t="s">
         <v>46</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -1304,27 +1400,27 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A5" s="27"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="36" t="s">
-        <v>102</v>
+      <c r="C5" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="39" t="s">
         <v>55</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="42" t="s">
         <v>37</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>34</v>
@@ -1340,27 +1436,30 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A6" s="27"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>106</v>
+      <c r="G6" s="39" t="s">
+        <v>161</v>
       </c>
       <c r="H6" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>109</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>47</v>
@@ -1368,7 +1467,7 @@
       <c r="K6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M6" s="9" t="s">
@@ -1376,23 +1475,23 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="5" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A7" s="28"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="37" t="s">
-        <v>103</v>
+      <c r="C7" s="38" t="s">
+        <v>104</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="40" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="39"/>
+      <c r="G7" s="40"/>
       <c r="H7" s="11" t="s">
         <v>21</v>
       </c>
@@ -1405,121 +1504,121 @@
       <c r="K7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="39" t="s">
+      <c r="L7" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="M7" s="39" t="s">
+      <c r="M7" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="25"/>
+      <c r="N7" s="26"/>
     </row>
     <row r="8" spans="1:14" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A8" s="49" t="s">
-        <v>116</v>
+      <c r="A8" s="50" t="s">
+        <v>117</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="46" t="s">
-        <v>102</v>
+      <c r="C8" s="47" t="s">
+        <v>103</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="H8" s="43" t="s">
+      <c r="G8" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="H8" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="21"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="22"/>
       <c r="N8" s="9"/>
     </row>
     <row r="9" spans="1:14" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A9" s="27"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="47"/>
+      <c r="C9" s="48"/>
       <c r="D9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="38" t="s">
-        <v>113</v>
-      </c>
-      <c r="H9" s="44"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="21"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="H9" s="45"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="22"/>
       <c r="N9" s="9"/>
     </row>
     <row r="10" spans="1:14" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A10" s="27"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="47"/>
+      <c r="C10" s="48"/>
       <c r="D10" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="42"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="21"/>
+      <c r="F10" s="43"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="22"/>
       <c r="N10" s="9" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A11" s="28"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="48"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="34"/>
+      <c r="F11" s="35"/>
       <c r="G11" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="H11" s="45"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="22"/>
+        <v>116</v>
+      </c>
+      <c r="H11" s="46"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="23"/>
       <c r="M11" s="15"/>
       <c r="N11" s="11"/>
     </row>
     <row r="12" spans="1:14" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="27" t="s">
         <v>68</v>
       </c>
       <c r="B12" s="13" t="s">
@@ -1528,7 +1627,7 @@
       <c r="D12" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="39" t="s">
         <v>70</v>
       </c>
       <c r="F12" s="6" t="s">
@@ -1548,14 +1647,14 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A13" s="27"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="13" t="s">
         <v>64</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="39" t="s">
         <v>70</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -1575,14 +1674,14 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A14" s="27"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="13" t="s">
         <v>65</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="39" t="s">
         <v>90</v>
       </c>
       <c r="F14" s="6" t="s">
@@ -1605,20 +1704,20 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A15" s="27"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="13" t="s">
         <v>66</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="41" t="s">
         <v>39</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G15" s="40"/>
+      <c r="G15" s="41"/>
       <c r="I15" s="6" t="s">
         <v>83</v>
       </c>
@@ -1630,21 +1729,21 @@
       </c>
     </row>
     <row r="16" spans="1:14" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A16" s="28"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="37"/>
+      <c r="C16" s="38"/>
       <c r="D16" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="39" t="s">
+      <c r="E16" s="40" t="s">
         <v>39</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="G16" s="39"/>
+      <c r="G16" s="40"/>
       <c r="H16" s="11" t="s">
         <v>88</v>
       </c>
@@ -1659,29 +1758,29 @@
       </c>
       <c r="L16" s="10"/>
       <c r="M16" s="11"/>
-      <c r="N16" s="25"/>
+      <c r="N16" s="26"/>
     </row>
     <row r="17" spans="1:14" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="50" t="s">
         <v>121</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C17" s="36" t="s">
         <v>118</v>
       </c>
+      <c r="C17" s="37" t="s">
+        <v>119</v>
+      </c>
       <c r="D17" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E17" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="F17" s="38" t="s">
+      <c r="E17" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="G17" s="38" t="s">
-        <v>132</v>
+      <c r="G17" s="39" t="s">
+        <v>153</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>131</v>
@@ -1697,11 +1796,11 @@
       </c>
     </row>
     <row r="18" spans="1:14" s="5" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A18" s="50"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="38" t="s">
         <v>127</v>
       </c>
       <c r="D18" s="10" t="s">
@@ -1718,13 +1817,133 @@
       <c r="K18" s="11"/>
       <c r="L18" s="10"/>
       <c r="M18" s="11"/>
-      <c r="N18" s="25" t="s">
+      <c r="N18" s="26" t="s">
         <v>130</v>
       </c>
     </row>
+    <row r="19" spans="1:14" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A19" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="F19" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="G19" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A20" s="28"/>
+      <c r="B20" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="N20" s="19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A21" s="28"/>
+      <c r="B21" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="N21" s="19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A22" s="28"/>
+      <c r="B22" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="F22" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="G22" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="N22" s="19" t="s">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A22"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="I1:K1"/>

</xml_diff>